<commit_message>
Merging main with existing branch
Tried merging both branches, error message still occurring.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT-Tr/Jasleen/RTFS_All_Countries.xlsx
+++ b/Inputs/_MasterFiles/FTT-Tr/Jasleen/RTFS_All_Countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\FTT\FTT_StandAlone\Inputs\_MasterFiles\FTT-Tr\Jasleen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb614170\FTT_StandAlone\Inputs\_MasterFiles\FTT-Tr\Jasleen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41BF0A1-106B-4700-A1C6-851C4942AF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F414DD52-06A1-4AE3-B353-5A5D94DBD80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A4F93CB-2A52-4596-A96F-B60626721FD0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6A4F93CB-2A52-4596-A96F-B60626721FD0}"/>
   </bookViews>
   <sheets>
     <sheet name="RTFS" sheetId="1" r:id="rId1"/>
@@ -896,42 +896,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4DC626-84ED-4583-9E91-CC0F97CC194C}">
   <dimension ref="A1:AA72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C71" sqref="C71:AA71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="23" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1180,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1263,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1346,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1512,7 +1513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1595,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1678,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1761,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2010,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -2176,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -2259,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -2342,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2425,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2508,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -2591,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -2674,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -2757,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2840,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2923,7 +2924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -3006,7 +3007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -3089,7 +3090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -3172,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -3255,7 +3256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -3338,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -3421,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -3504,7 +3505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -3587,7 +3588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -3670,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -3753,7 +3754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -3836,7 +3837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -3919,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -4002,7 +4003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -4085,7 +4086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>64</v>
       </c>
@@ -4168,7 +4169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>65</v>
       </c>
@@ -4251,7 +4252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -4334,7 +4335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>67</v>
       </c>
@@ -4417,7 +4418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -4500,7 +4501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -4583,7 +4584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -4666,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>71</v>
       </c>
@@ -4749,7 +4750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -4832,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>73</v>
       </c>
@@ -4915,7 +4916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -4998,7 +4999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>75</v>
       </c>
@@ -5081,7 +5082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -5164,7 +5165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>77</v>
       </c>
@@ -5247,7 +5248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -5330,7 +5331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -5413,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -5496,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>80</v>
       </c>
@@ -5579,7 +5580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>81</v>
       </c>
@@ -5662,7 +5663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -5745,7 +5746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>83</v>
       </c>
@@ -5828,7 +5829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>84</v>
       </c>
@@ -5911,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -5994,7 +5995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -6077,7 +6078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>87</v>
       </c>
@@ -6160,7 +6161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -6243,7 +6244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -6326,7 +6327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>90</v>
       </c>
@@ -6409,7 +6410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>91</v>
       </c>
@@ -6492,7 +6493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>92</v>
       </c>
@@ -6575,7 +6576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>93</v>
       </c>
@@ -6658,7 +6659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>94</v>
       </c>
@@ -6741,7 +6742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>95</v>
       </c>
@@ -6824,7 +6825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>96</v>
       </c>

</xml_diff>